<commit_message>
create nta specific desire lines
</commit_message>
<xml_diff>
--- a/data/nyc_2010_census_tract_nta_equiv.xlsx
+++ b/data/nyc_2010_census_tract_nta_equiv.xlsx
@@ -30,22 +30,22 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13893" uniqueCount="1818">
   <si>
-    <t xml:space="preserve">borough-name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">county-code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">borough-code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Census-tract</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nta-code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nta-name</t>
+    <t xml:space="preserve">borough_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">county_code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">borough_code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">census_tract</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nta_code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nta_name</t>
   </si>
   <si>
     <t xml:space="preserve">Bronx</t>
@@ -5691,23 +5691,6 @@
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
     <cellStyle name="Normal 2" xfId="20"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF7F7F7"/>
-          <bgColor rgb="FF272727"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -5779,12 +5762,12 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
+      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.29"/>

</xml_diff>